<commit_message>
export excel | revisi seeder partisipasi
</commit_message>
<xml_diff>
--- a/public/assets/excel/daftar_partisipan.xlsx
+++ b/public/assets/excel/daftar_partisipan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\esertif-vokasi\public\assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B43FF9F-4C57-4176-8C47-B8B1101AFAE6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAE1AB7A-9D3D-463C-B19A-BC38DCE6E114}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D7E385F6-A802-4739-8B79-7396189CA014}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{D7E385F6-A802-4739-8B79-7396189CA014}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Partisipan" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="80">
   <si>
     <t>NIM</t>
   </si>
@@ -289,6 +289,9 @@
   </si>
   <si>
     <t>151811513004</t>
+  </si>
+  <si>
+    <t>Pemateri</t>
   </si>
 </sst>
 </file>
@@ -747,7 +750,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD8F0937-4B77-4611-854A-AFE494D2C7D1}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
@@ -823,10 +826,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7E30172-5642-4471-ADA7-489DAF27C9FB}">
-  <dimension ref="A1:L143"/>
+  <dimension ref="A1:L147"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E142" sqref="E142"/>
+    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
+      <selection activeCell="F131" sqref="F131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1121,114 +1124,119 @@
         <v>23</v>
       </c>
     </row>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>9</v>
+      </c>
+    </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B31" s="3" t="s">
+      <c r="C31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B35" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B33" s="3" t="s">
+    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B37" s="3" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B35" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B37" s="5" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B39" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B41" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B43" s="5" t="s">
         <v>28</v>
-      </c>
-    </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C40" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C41" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C42" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C43" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="44" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C44" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
     </row>
     <row r="45" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C45" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C46" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C47" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C48" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C49" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B47" s="5" t="s">
+    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B51" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B49" s="5" t="s">
+    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B53" s="5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C50" t="s">
+    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C54" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C51" t="s">
+    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C55" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C52" t="s">
+    <row r="56" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C56" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C53" t="s">
+    <row r="57" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C57" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B55" s="5" t="s">
+    <row r="59" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B59" s="5" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="57" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B57" s="5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="58" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C58" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="59" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C59" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="61" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B61" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="62" spans="2:3" x14ac:dyDescent="0.25">
@@ -1243,7 +1251,7 @@
     </row>
     <row r="65" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B65" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="66" spans="2:3" x14ac:dyDescent="0.25">
@@ -1258,217 +1266,217 @@
     </row>
     <row r="69" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B69" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="70" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C70" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="71" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C71" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="73" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B73" s="5" t="s">
         <v>42</v>
-      </c>
-    </row>
-    <row r="71" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B71" s="5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="72" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C72" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="73" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C73" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="75" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B75" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="76" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C76" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="77" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B77" s="5" t="s">
-        <v>45</v>
+      <c r="C77" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="79" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B79" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="81" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B81" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="83" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B83" s="5" t="s">
         <v>46</v>
-      </c>
-    </row>
-    <row r="80" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C80" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="81" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C81" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="82" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C82" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="83" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C83" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="84" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C84" t="s">
-        <v>33</v>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="85" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C85" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="86" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B86" s="5" t="s">
-        <v>48</v>
+      <c r="C86" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="87" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C87" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="88" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C88" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="89" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C89" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="90" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C90" t="s">
-        <v>32</v>
+      <c r="B90" s="5" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="91" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C91" t="s">
-        <v>33</v>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="92" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C92" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="93" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B93" s="5" t="s">
-        <v>49</v>
+      <c r="C93" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="94" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C94" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
     </row>
     <row r="95" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C95" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="97" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B97" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="98" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C98" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="99" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C99" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="96" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C96" t="s">
+    <row r="100" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C100" t="s">
         <v>52</v>
-      </c>
-    </row>
-    <row r="98" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B98" s="5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="100" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B100" s="5" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="102" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B102" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="104" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B104" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="106" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B106" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="108" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B108" s="5" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="109" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C109" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="110" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C110" t="s">
-        <v>60</v>
+      <c r="B110" s="5" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="112" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B112" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="113" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C113" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="114" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C114" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="116" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B116" s="5" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="114" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B114" s="5" t="s">
+    <row r="118" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B118" s="5" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="116" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B116" s="5" t="s">
+    <row r="120" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B120" s="5" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="118" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B118" s="5" t="s">
+    <row r="122" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B122" s="5" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="120" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B120" s="5" t="s">
+    <row r="124" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B124" s="5" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="122" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B122" s="5" t="s">
+    <row r="126" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B126" s="5" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="124" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B124" s="5" t="s">
+    <row r="128" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B128" s="5" t="s">
         <v>67</v>
-      </c>
-    </row>
-    <row r="126" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B126" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="128" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B128" s="5" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="130" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B130" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="132" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B132" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="134" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B134" s="5" t="s">
         <v>70</v>
-      </c>
-    </row>
-    <row r="131" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C131" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="132" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C132" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="134" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B134" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="135" spans="2:3" x14ac:dyDescent="0.25">
@@ -1482,27 +1490,42 @@
       </c>
     </row>
     <row r="138" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B138" s="5" t="s">
-        <v>73</v>
+      <c r="B138" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="139" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C139" t="s">
-        <v>31</v>
+        <v>71</v>
       </c>
     </row>
     <row r="140" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C140" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="142" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B142" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="143" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C143" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="144" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C144" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="141" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C141" t="s">
+    <row r="145" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C145" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="143" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B143" s="5" t="s">
+    <row r="147" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B147" s="5" t="s">
         <v>74</v>
       </c>
     </row>

</xml_diff>